<commit_message>
Berisi tentang pembagian job desc team
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\Data Kuliah\SMT 7\Mechine Learning\Tubes\tubesPrak_171-173\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C1826B-50B3-470E-B59D-0B10EE4EA48D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA8F5A1-E1A7-4452-B3FE-307A494F059C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="11490" xr2:uid="{4DF276D9-079A-4F51-A4F0-0A87F36BF914}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t xml:space="preserve">NO </t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Model 1</t>
-  </si>
-  <si>
-    <t>Ongoing</t>
   </si>
   <si>
     <t>27 Ot 2021</t>
@@ -479,7 +476,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,10 +576,12 @@
       <c r="E4" s="3">
         <v>44496</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="3">
+        <v>44496</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -596,12 +595,14 @@
         <v>44494</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44496</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>